<commit_message>
fixed: index 2 is fixed
</commit_message>
<xml_diff>
--- a/Data/twistedpendant_products.xlsx
+++ b/Data/twistedpendant_products.xlsx
@@ -620,7 +620,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/185_dfcac9ca-75dc-45e8-b152-83cc41a4008e.jpg; //twistedpendant.com/cdn/shop/files/170_8f7870f1-f1d6-44cd-baa6-499fd7837645.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/185_dfcac9ca-75dc-45e8-b152-83cc41a4008e.jpg; https://twistedpendant.com/cdn/shop/files/170_8f7870f1-f1d6-44cd-baa6-499fd7837645.jpg; https://twistedpendant.com/cdn/shop/files/169_996a5e8e-5100-42a9-94a8-85bf182166e1.jpg</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -651,11 +651,11 @@
       </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/129_3b03015d-eb85-4937-8418-ff9eccba1608.jpg; //twistedpendant.com/cdn/shop/files/274_5f2cbaed-3427-48bf-80a5-8809ae73ea6b.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/129_3b03015d-eb85-4937-8418-ff9eccba1608.jpg; https://twistedpendant.com/cdn/shop/files/274_5f2cbaed-3427-48bf-80a5-8809ae73ea6b.jpg; https://twistedpendant.com/cdn/shop/files/131_4adc784c-e64a-427a-8b0a-ee5d95e522f3.jpg</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -750,11 +750,11 @@
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -841,7 +841,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/336.jpg; //twistedpendant.com/cdn/shop/files/340.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/336.jpg; https://twistedpendant.com/cdn/shop/files/340.jpg; https://twistedpendant.com/cdn/shop/files/341.jpg</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/5_73de58e2-3d40-465c-853c-4d63f6e09e53.jpg; //twistedpendant.com/cdn/shop/files/112_55f6d841-14ee-46a2-af27-d7d61bdcd1dc.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/5_73de58e2-3d40-465c-853c-4d63f6e09e53.jpg; https://twistedpendant.com/cdn/shop/files/112_55f6d841-14ee-46a2-af27-d7d61bdcd1dc.jpg; https://twistedpendant.com/cdn/shop/files/6_36e8c3ab-8ce2-4af4-ae8f-e2d5dc2755cd.jpg</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -990,11 +990,11 @@
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/183_af6cc016-54e8-4348-afb1-a1067b7bf123.jpg; //twistedpendant.com/cdn/shop/files/2_87dc4193-f805-4a60-8506-84df87edb95c.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/183_af6cc016-54e8-4348-afb1-a1067b7bf123.jpg; https://twistedpendant.com/cdn/shop/files/2_87dc4193-f805-4a60-8506-84df87edb95c.png; https://twistedpendant.com/cdn/shop/files/3_1fc8bba8-96ad-4e41-8348-0ce9ad562c53.png</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1105,11 +1105,11 @@
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/42_715111ca-278c-4b36-996c-afc608b333ee.jpg; //twistedpendant.com/cdn/shop/files/26_ba0b1ac8-805c-4505-8ea9-14e7d06074e5.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/42_715111ca-278c-4b36-996c-afc608b333ee.jpg; https://twistedpendant.com/cdn/shop/files/26_ba0b1ac8-805c-4505-8ea9-14e7d06074e5.jpg; https://twistedpendant.com/cdn/shop/files/21_e12592a5-b7f5-474b-b3f2-4506fc4e199d.jpg</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/72_668fe5d2-b090-478c-8376-87e86fcf4f99.jpg; //twistedpendant.com/cdn/shop/files/4_c9733a97-0b9f-4e8c-93fb-b21fc86dca7d.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/72_668fe5d2-b090-478c-8376-87e86fcf4f99.jpg; https://twistedpendant.com/cdn/shop/files/4_c9733a97-0b9f-4e8c-93fb-b21fc86dca7d.jpg; https://twistedpendant.com/cdn/shop/products/6_a3c32487-1354-41c7-b328-421e19101f4d.png</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1314,11 +1314,11 @@
       </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/116_ed1d648a-501d-476e-9fad-7439b11ae286.jpg; //twistedpendant.com/cdn/shop/files/144_a2661131-978d-4996-82e3-ea522a1decd2.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/116_ed1d648a-501d-476e-9fad-7439b11ae286.jpg; https://twistedpendant.com/cdn/shop/files/144_a2661131-978d-4996-82e3-ea522a1decd2.jpg; https://twistedpendant.com/cdn/shop/files/141_b2e929ef-873b-420e-8502-cab6df566ca3.jpg</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/127_6d03e89f-b61c-4ef0-994f-b1b0f94a6418.jpg; //twistedpendant.com/cdn/shop/files/2_2_1633a3a7-386f-46af-a669-98811995b734.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/127_6d03e89f-b61c-4ef0-994f-b1b0f94a6418.jpg; https://twistedpendant.com/cdn/shop/files/2_2_1633a3a7-386f-46af-a669-98811995b734.jpg; https://twistedpendant.com/cdn/shop/files/1_756288c2-817c-4e66-a29a-87ba5cfdc95b.jpg</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1541,11 +1541,11 @@
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/161_7290cd13-5a6d-40b2-90d5-bad64b77e8a3.jpg; //twistedpendant.com/cdn/shop/files/MOSS_AGATE_SQUARE.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/161_7290cd13-5a6d-40b2-90d5-bad64b77e8a3.jpg; https://twistedpendant.com/cdn/shop/files/MOSS_AGATE_SQUARE.jpg; https://twistedpendant.com/cdn/shop/files/116_9a709c88-2d57-4376-86d1-4d8fdad5a643.jpg</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1659,11 +1659,11 @@
       </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/179_a183d59b-0432-4fe2-81f6-fc182eab46a6.jpg; //twistedpendant.com/cdn/shop/files/4_2bb654f2-56ea-4bbf-afb6-c64a5e35a05b.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/179_a183d59b-0432-4fe2-81f6-fc182eab46a6.jpg; https://twistedpendant.com/cdn/shop/files/4_2bb654f2-56ea-4bbf-afb6-c64a5e35a05b.jpg; https://twistedpendant.com/cdn/shop/files/1_fa3ea521-223e-467a-bd04-0f7f648453a6.jpg</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1772,11 +1772,11 @@
       </c>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/128_51ef4415-eafb-4895-9069-874456d5eb47.jpg; //twistedpendant.com/cdn/shop/files/268.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/128_51ef4415-eafb-4895-9069-874456d5eb47.jpg; https://twistedpendant.com/cdn/shop/files/268.jpg; https://twistedpendant.com/cdn/shop/files/259.jpg</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1871,11 +1871,11 @@
       </c>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/335.jpg; //twistedpendant.com/cdn/shop/files/Untitled_design_22.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/335.jpg; https://twistedpendant.com/cdn/shop/files/Untitled_design_22.jpg; https://twistedpendant.com/cdn/shop/files/339.jpg</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/41_5df21682-8d32-4fbf-8ed1-15a8444a6fb7.jpg; //twistedpendant.com/cdn/shop/files/38_42d2b73b-2616-44be-a53c-11e40c0ab192.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/41_5df21682-8d32-4fbf-8ed1-15a8444a6fb7.jpg; https://twistedpendant.com/cdn/shop/files/38_42d2b73b-2616-44be-a53c-11e40c0ab192.jpg; https://twistedpendant.com/cdn/shop/files/23_733e8323-67b8-4db6-943f-1b75d915a2fe.jpg</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2090,11 +2090,11 @@
       </c>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/133_1fdcbcb0-8d4d-458b-aabc-ec018ead30c0.jpg; //twistedpendant.com/cdn/shop/files/14_8b6342b2-d12b-4a74-b92f-e72b6edcdcd5.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/133_1fdcbcb0-8d4d-458b-aabc-ec018ead30c0.jpg; https://twistedpendant.com/cdn/shop/files/14_8b6342b2-d12b-4a74-b92f-e72b6edcdcd5.jpg; https://twistedpendant.com/cdn/shop/files/9_34fb98f8-4663-48f6-bf04-4f11c3441125.jpg</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -2202,11 +2202,11 @@
       </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/106_b192f9d1-e5bc-4b42-becc-a5251785b75b.jpg; //twistedpendant.com/cdn/shop/files/MALACHITE_-_OVAL_2.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/106_b192f9d1-e5bc-4b42-becc-a5251785b75b.jpg; https://twistedpendant.com/cdn/shop/files/MALACHITE_-_OVAL_2.jpg; https://twistedpendant.com/cdn/shop/files/4_f0bfac33-0ea0-4f92-a42b-cead89b9c562.jpg</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -2320,11 +2320,11 @@
       </c>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/139_30317fc1-772e-4535-aecf-e83e55c560ff.jpg; //twistedpendant.com/cdn/shop/files/11_31b0c833-1ed7-41c5-851f-3647e6706cd4.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/139_30317fc1-772e-4535-aecf-e83e55c560ff.jpg; https://twistedpendant.com/cdn/shop/files/11_31b0c833-1ed7-41c5-851f-3647e6706cd4.jpg; https://twistedpendant.com/cdn/shop/files/3_9084ad01-d709-4cde-9fed-5b4c3c7601d1.jpg</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2416,11 +2416,11 @@
       </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/78_a6cbbc2f-f319-4449-9b53-27706c89887b.jpg; //twistedpendant.com/cdn/shop/products/5_0734f12b-0adc-4882-9e1b-9b2aa010eceb.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/78_a6cbbc2f-f319-4449-9b53-27706c89887b.jpg; https://twistedpendant.com/cdn/shop/products/5_0734f12b-0adc-4882-9e1b-9b2aa010eceb.png; https://twistedpendant.com/cdn/shop/files/3_3384d4ac-cc52-4778-aa1f-3f0d07e446d7.png</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2530,11 +2530,11 @@
       </c>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/146_9ff3afe4-c7c0-4d85-8be1-ce7335cfa309.jpg; //twistedpendant.com/cdn/shop/files/117.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/146_9ff3afe4-c7c0-4d85-8be1-ce7335cfa309.jpg; https://twistedpendant.com/cdn/shop/files/117.png; https://twistedpendant.com/cdn/shop/files/106.png</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/108_deec515e-d357-478d-bd20-3c9d62dcb055.jpg; //twistedpendant.com/cdn/shop/files/3_59967c9f-bcdb-40f9-a91a-b75e2b421abf.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/108_deec515e-d357-478d-bd20-3c9d62dcb055.jpg; https://twistedpendant.com/cdn/shop/files/3_59967c9f-bcdb-40f9-a91a-b75e2b421abf.jpg; https://twistedpendant.com/cdn/shop/files/6_7db314bb-31fd-4817-a462-ba49401c1384.jpg</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2760,11 +2760,11 @@
       </c>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/184_51e54ad2-cb84-4778-ab40-8f0437530621.jpg; //twistedpendant.com/cdn/shop/products/OnyxRingV1.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/184_51e54ad2-cb84-4778-ab40-8f0437530621.jpg; https://twistedpendant.com/cdn/shop/products/OnyxRingV1.png; https://twistedpendant.com/cdn/shop/products/1_4f359cc4-03f7-4d53-bf03-6dd96693b794.png</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/116_a3b810a0-e560-403f-9a1b-6e66db7ded97.jpg; //twistedpendant.com/cdn/shop/products/image_4afd573f-f29d-42fb-b950-80d17bb268ba.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/116_a3b810a0-e560-403f-9a1b-6e66db7ded97.jpg; https://twistedpendant.com/cdn/shop/products/image_4afd573f-f29d-42fb-b950-80d17bb268ba.jpg; https://twistedpendant.com/cdn/shop/products/2_5383de68-db49-4e92-9100-fa7eaa2d1af7.jpg</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2987,11 +2987,11 @@
       </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/76_9aebe509-3fc2-415c-ba0f-4e2c0ebc3ead.jpg; //twistedpendant.com/cdn/shop/files/image_db62be5b-284c-4569-a1fb-b5a2ce68822a.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/76_9aebe509-3fc2-415c-ba0f-4e2c0ebc3ead.jpg; https://twistedpendant.com/cdn/shop/files/image_db62be5b-284c-4569-a1fb-b5a2ce68822a.jpg; https://twistedpendant.com/cdn/shop/files/image_1424f5ad-cd61-46d3-8f2d-1fc10ce1d1fb.jpg</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -3101,11 +3101,11 @@
       </c>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/35_4d43a7a4-729a-40dc-8bae-b4f89e1e31e8.jpg; //twistedpendant.com/cdn/shop/files/4_b9dba399-b833-4472-b39b-422b43f144da.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/35_4d43a7a4-729a-40dc-8bae-b4f89e1e31e8.jpg; https://twistedpendant.com/cdn/shop/files/4_b9dba399-b833-4472-b39b-422b43f144da.jpg; https://twistedpendant.com/cdn/shop/files/3_2f4db097-f05d-4840-bdbb-4eaed304762a.jpg</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -3215,11 +3215,11 @@
       </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/177_7aa4ffdd-9533-41cc-a04b-9e9b92a62765.jpg; //twistedpendant.com/cdn/shop/files/186_c89fd354-eb76-4e5e-b671-d0de1ce2149e.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/177_7aa4ffdd-9533-41cc-a04b-9e9b92a62765.jpg; https://twistedpendant.com/cdn/shop/files/186_c89fd354-eb76-4e5e-b671-d0de1ce2149e.jpg; https://twistedpendant.com/cdn/shop/files/3_9bf99300-71d0-4be8-bc88-6e1260327465.png</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -3327,11 +3327,11 @@
       </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/115_14b60c9e-6b14-430e-bdba-2b8e4afcf576.jpg; //twistedpendant.com/cdn/shop/files/137_c6eede69-7e97-4997-877b-e82cd3cc025a.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/115_14b60c9e-6b14-430e-bdba-2b8e4afcf576.jpg; https://twistedpendant.com/cdn/shop/files/137_c6eede69-7e97-4997-877b-e82cd3cc025a.jpg; https://twistedpendant.com/cdn/shop/files/SUGILITE_-_OVAL.jpg</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -3443,11 +3443,11 @@
       </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/165_8fc04e29-402d-46d8-9777-c92bbc031b5f.jpg; //twistedpendant.com/cdn/shop/files/67_66b89de8-2c9f-47e3-8699-823b78143a9d.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/165_8fc04e29-402d-46d8-9777-c92bbc031b5f.jpg; https://twistedpendant.com/cdn/shop/files/67_66b89de8-2c9f-47e3-8699-823b78143a9d.jpg; https://twistedpendant.com/cdn/shop/files/117_4d41106d-6c4f-4f91-9d40-c01f3d8036be.jpg</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -3561,11 +3561,11 @@
       </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3648,7 +3648,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/107_12c5e734-22ca-4206-867d-fb30255796fc.jpg; //twistedpendant.com/cdn/shop/files/4_18947ddb-b539-45b6-9120-003a68bd7a37.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/107_12c5e734-22ca-4206-867d-fb30255796fc.jpg; https://twistedpendant.com/cdn/shop/files/4_18947ddb-b539-45b6-9120-003a68bd7a37.jpg; https://twistedpendant.com/cdn/shop/files/MALACHITE_-_OVAL.jpg</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -3679,11 +3679,11 @@
       </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/76_dc1078da-75cb-4ae4-926d-deb0e2dc2d05.jpg; //twistedpendant.com/cdn/shop/files/4_fd3261cf-530f-4fe2-a423-dac9c851dc8c.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/76_dc1078da-75cb-4ae4-926d-deb0e2dc2d05.jpg; https://twistedpendant.com/cdn/shop/files/4_fd3261cf-530f-4fe2-a423-dac9c851dc8c.png; https://twistedpendant.com/cdn/shop/products/2_32af18a4-f020-478a-8d94-e62255238dc8.png</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -3794,11 +3794,11 @@
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/182.jpg; //twistedpendant.com/cdn/shop/files/10_cea2aa1a-38e7-4fb8-9620-852442435e1b.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/182.jpg; https://twistedpendant.com/cdn/shop/files/10_cea2aa1a-38e7-4fb8-9620-852442435e1b.jpg; https://twistedpendant.com/cdn/shop/files/189_d25fd493-cdb9-4394-8842-875f0a518370.jpg</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -3907,11 +3907,11 @@
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/130_9a7a3509-30ec-49bd-9e48-83468cb2f422.jpg; //twistedpendant.com/cdn/shop/files/109_ba7e3945-b8a6-4ee2-b731-ddf05c6c5ea0.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/130_9a7a3509-30ec-49bd-9e48-83468cb2f422.jpg; https://twistedpendant.com/cdn/shop/files/109_ba7e3945-b8a6-4ee2-b731-ddf05c6c5ea0.jpg; https://twistedpendant.com/cdn/shop/files/119_7e7d4b05-539d-48e3-b1ae-1b7ac7e79889.jpg</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -4020,11 +4020,11 @@
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/4_85935925-3b29-4954-9ef7-3880ab1f51d8.jpg; //twistedpendant.com/cdn/shop/files/3_5180c444-3597-4a5a-beb8-a0b6969fd870.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/4_85935925-3b29-4954-9ef7-3880ab1f51d8.jpg; https://twistedpendant.com/cdn/shop/files/3_5180c444-3597-4a5a-beb8-a0b6969fd870.png; https://twistedpendant.com/cdn/shop/files/Untitled_design-30_a86950a0-cf2a-43e4-aec0-d8e85b156c2e.jpg</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -4132,11 +4132,11 @@
       </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4215,7 +4215,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/80_339d5c53-d14e-4560-a34a-8630a1f85802.jpg; //twistedpendant.com/cdn/shop/products/7_b41918aa-9e23-48ae-89c8-2330e4cf3f21.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/80_339d5c53-d14e-4560-a34a-8630a1f85802.jpg; https://twistedpendant.com/cdn/shop/products/7_b41918aa-9e23-48ae-89c8-2330e4cf3f21.png; https://twistedpendant.com/cdn/shop/products/dsc6739_dad9591f-eb57-47d8-a98d-ba9c42bee89a.jpg</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4329,7 +4329,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/17_fc3c34ca-ade5-4b6b-8d17-5d30bab35516.jpg; //twistedpendant.com/cdn/shop/files/11_e0be0d06-c906-44f1-ad49-5d3b9ae0edb2.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/17_fc3c34ca-ade5-4b6b-8d17-5d30bab35516.jpg; https://twistedpendant.com/cdn/shop/files/11_e0be0d06-c906-44f1-ad49-5d3b9ae0edb2.jpg; https://twistedpendant.com/cdn/shop/files/9_4c1a3c2d-06c6-4d09-898e-054f8f0c8a25.jpg</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -4364,7 +4364,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/55_984accbb-6b5c-41d5-b706-1dbc9c29f990.jpg; //twistedpendant.com/cdn/shop/files/1_5e15920e-b0af-4710-9744-004ece6ab480.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/55_984accbb-6b5c-41d5-b706-1dbc9c29f990.jpg; https://twistedpendant.com/cdn/shop/files/1_5e15920e-b0af-4710-9744-004ece6ab480.png; https://twistedpendant.com/cdn/shop/files/Vortex-Silver.jpg</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -4480,7 +4480,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/132_a965ec87-8f35-42c2-80c2-e1123f24ca03.jpg; //twistedpendant.com/cdn/shop/files/11_e03a1c6c-5f39-44b6-ae5a-3839b635ea98.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/132_a965ec87-8f35-42c2-80c2-e1123f24ca03.jpg; https://twistedpendant.com/cdn/shop/files/11_e03a1c6c-5f39-44b6-ae5a-3839b635ea98.jpg; https://twistedpendant.com/cdn/shop/files/9_34fb98f8-4663-48f6-bf04-4f11c3441125.jpg</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -4588,11 +4588,11 @@
       </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/138_77137b7d-4036-4fad-8c63-c0a358f45bce.jpg; //twistedpendant.com/cdn/shop/files/13_14dcc54c-165d-4e79-8e9b-f88d3e59bd54.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/138_77137b7d-4036-4fad-8c63-c0a358f45bce.jpg; https://twistedpendant.com/cdn/shop/files/13_14dcc54c-165d-4e79-8e9b-f88d3e59bd54.jpg; https://twistedpendant.com/cdn/shop/files/22_6501146d-9fda-4428-a624-566e3ab519c0.jpg</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -4686,11 +4686,11 @@
       </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4753,7 +4753,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/77_a8b410d2-d2ca-4f22-ad7e-2a68a8fade60.jpg; //twistedpendant.com/cdn/shop/products/2_5f5d8bb8-42dc-4bb0-ba82-4f10c65baf3e.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/77_a8b410d2-d2ca-4f22-ad7e-2a68a8fade60.jpg; https://twistedpendant.com/cdn/shop/products/2_5f5d8bb8-42dc-4bb0-ba82-4f10c65baf3e.png; https://twistedpendant.com/cdn/shop/products/1_e3aa72ed-de09-4c32-9d9c-42d05a71d668.png</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -4784,11 +4784,11 @@
       </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/140_e1c1f327-786d-44c4-acde-7fe4b6a0f39e.jpg; //twistedpendant.com/cdn/shop/files/111.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/140_e1c1f327-786d-44c4-acde-7fe4b6a0f39e.jpg; https://twistedpendant.com/cdn/shop/files/111.png; https://twistedpendant.com/cdn/shop/files/113.png</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -4896,11 +4896,11 @@
       </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/111_2070358d-ea51-4fa5-a46b-bb33ab64e6a0.jpg; //twistedpendant.com/cdn/shop/files/BLUE_LACE_-_OVAL.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/111_2070358d-ea51-4fa5-a46b-bb33ab64e6a0.jpg; https://twistedpendant.com/cdn/shop/files/BLUE_LACE_-_OVAL.jpg; https://twistedpendant.com/cdn/shop/files/126_764c51f4-8ee7-441c-b0b4-76f4b2605f27.jpg</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -5014,11 +5014,11 @@
       </c>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/60_58744951-1cb0-4788-9feb-de7d0cd05c3b.jpg; //twistedpendant.com/cdn/shop/files/1_3793fc2b-e65e-4050-9c93-227e85a6252d.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/60_58744951-1cb0-4788-9feb-de7d0cd05c3b.jpg; https://twistedpendant.com/cdn/shop/files/1_3793fc2b-e65e-4050-9c93-227e85a6252d.png; https://twistedpendant.com/cdn/shop/files/IMG_9558.jpg</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -5113,11 +5113,11 @@
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/134_bae40427-e22a-4e2f-b23a-61f12cc080cb.jpg; //twistedpendant.com/cdn/shop/files/1_c03819af-001d-4b82-bf2f-551265876a7a.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/134_bae40427-e22a-4e2f-b23a-61f12cc080cb.jpg; https://twistedpendant.com/cdn/shop/files/1_c03819af-001d-4b82-bf2f-551265876a7a.jpg; https://twistedpendant.com/cdn/shop/files/2_3b27d1a1-b289-441e-88f4-8fb3da477e78.jpg</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -5226,11 +5226,11 @@
       </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/182_fe4fcf03-fea5-4358-afed-59d6abe2c443.jpg; //twistedpendant.com/cdn/shop/files/9_598d3826-392d-4c5e-b6de-f7538e4bf400.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/182_fe4fcf03-fea5-4358-afed-59d6abe2c443.jpg; https://twistedpendant.com/cdn/shop/files/9_598d3826-392d-4c5e-b6de-f7538e4bf400.png; https://twistedpendant.com/cdn/shop/files/12_b2f2f2c9-2942-427f-b298-814ae7707afa.png</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -5325,11 +5325,11 @@
       </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5411,7 +5411,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/136_9e394a6b-9ba9-4321-a139-9c18a45a354b.jpg; //twistedpendant.com/cdn/shop/files/3_229b59ab-762d-42a5-b5e3-4fb5cceacf95.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/136_9e394a6b-9ba9-4321-a139-9c18a45a354b.jpg; https://twistedpendant.com/cdn/shop/files/3_229b59ab-762d-42a5-b5e3-4fb5cceacf95.png; https://twistedpendant.com/cdn/shop/files/8_a64e7850-4a18-41d2-9089-ef63a1ca3eba.png</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -5442,11 +5442,11 @@
       </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5528,7 +5528,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/135_4835c34c-f2d7-414c-9265-9e19d85c6fba.jpg; //twistedpendant.com/cdn/shop/files/1_61b33f61-1814-42db-bfa0-d3ca3387c461.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/135_4835c34c-f2d7-414c-9265-9e19d85c6fba.jpg; https://twistedpendant.com/cdn/shop/files/1_61b33f61-1814-42db-bfa0-d3ca3387c461.png; https://twistedpendant.com/cdn/shop/files/2_87205c3c-e6d5-4eba-9a2e-153605a433a9.png</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -5559,11 +5559,11 @@
       </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/110_f32d9a54-5cb7-4f82-bd70-345f4e353f4f.jpg; //twistedpendant.com/cdn/shop/files/159_2e32de38-dd25-482a-9478-979e32181368.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/110_f32d9a54-5cb7-4f82-bd70-345f4e353f4f.jpg; https://twistedpendant.com/cdn/shop/files/159_2e32de38-dd25-482a-9478-979e32181368.jpg; https://twistedpendant.com/cdn/shop/files/157_c2984b2d-4f9b-45d2-bbfa-726ada2142c1.jpg</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -5677,11 +5677,11 @@
       </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5762,7 +5762,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/183_2.jpg; //twistedpendant.com/cdn/shop/files/9_8484d11a-afe9-43a2-8dde-19900433b25d.png</t>
+          <t>https://twistedpendant.com/cdn/shop/files/183_2.jpg; https://twistedpendant.com/cdn/shop/files/9_8484d11a-afe9-43a2-8dde-19900433b25d.png; https://twistedpendant.com/cdn/shop/files/6_9e84aeec-8af3-425c-9f90-7736d337344b.png</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -5793,11 +5793,11 @@
       </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>//twistedpendant.com/cdn/shop/files/118_4cf249cd-307b-49b7-b2d5-be9954c17f14.jpg; //twistedpendant.com/cdn/shop/files/145_85041323-ed41-4f28-b449-21dd4af8c877.jpg</t>
+          <t>https://twistedpendant.com/cdn/shop/files/118_4cf249cd-307b-49b7-b2d5-be9954c17f14.jpg; https://twistedpendant.com/cdn/shop/files/145_85041323-ed41-4f28-b449-21dd4af8c877.jpg; https://twistedpendant.com/cdn/shop/files/SUGILITE_-_SQUARE.jpg</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -5914,7 +5914,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>men,ring</t>
+          <t>women,ring</t>
         </is>
       </c>
     </row>

</xml_diff>